<commit_message>
Dokumentation & Gantt update
</commit_message>
<xml_diff>
--- a/docs/210_Vorlage_GanttDiagramm.110.xlsx
+++ b/docs/210_Vorlage_GanttDiagramm.110.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="35">
   <si>
     <t>Nr.</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Realisation</t>
   </si>
   <si>
-    <t>32h / 24h</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
   </si>
   <si>
     <t>User Story</t>
-  </si>
-  <si>
-    <t>User Story ...</t>
   </si>
   <si>
     <r>
@@ -140,12 +134,39 @@
   <si>
     <t>Aaron Meier IST</t>
   </si>
+  <si>
+    <t>User Story 3</t>
+  </si>
+  <si>
+    <t>User Story 4</t>
+  </si>
+  <si>
+    <t>User Story 5</t>
+  </si>
+  <si>
+    <t>User Story 6</t>
+  </si>
+  <si>
+    <t>User Story 7</t>
+  </si>
+  <si>
+    <t>User Story 8</t>
+  </si>
+  <si>
+    <t>User Story 9</t>
+  </si>
+  <si>
+    <t>User Story 10</t>
+  </si>
+  <si>
+    <t>6h / 5h</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +221,13 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,7 +509,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
@@ -501,7 +529,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,19 +582,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,6 +595,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -589,16 +611,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -610,12 +632,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -625,18 +641,36 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
@@ -943,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK28"/>
+  <dimension ref="A1:BK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BR17" sqref="BR17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +990,7 @@
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17" style="22" customWidth="1"/>
+    <col min="6" max="6" width="17" style="21" customWidth="1"/>
     <col min="7" max="7" width="3.140625" style="5" customWidth="1"/>
     <col min="8" max="9" width="3.140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="3.7109375" style="8" bestFit="1" customWidth="1"/>
@@ -1005,110 +1039,92 @@
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="56">
+      <c r="F1" s="22"/>
+      <c r="G1" s="49">
         <v>7.03</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="56">
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="49">
         <v>8.0299999999999994</v>
       </c>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="56">
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="49">
         <v>9.0299999999999994</v>
       </c>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="56">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="49">
         <v>14.03</v>
       </c>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="56">
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="49">
         <v>15.03</v>
       </c>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="56">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="56">
-        <v>25.1</v>
-      </c>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="56">
-        <v>26.1</v>
-      </c>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="58"/>
-      <c r="AM1" s="56">
-        <v>27.2</v>
-      </c>
-      <c r="AN1" s="57"/>
-      <c r="AO1" s="57"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="56">
-        <v>1.2</v>
-      </c>
-      <c r="AR1" s="57"/>
-      <c r="AS1" s="57"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="56">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AV1" s="57"/>
-      <c r="AW1" s="57"/>
-      <c r="AX1" s="58"/>
-      <c r="AY1" s="56">
-        <v>3.2</v>
-      </c>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="57"/>
-      <c r="BB1" s="58"/>
-      <c r="BC1" s="56">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="BD1" s="57"/>
-      <c r="BE1" s="57"/>
-      <c r="BF1" s="58"/>
-      <c r="BG1" s="56">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="BH1" s="57"/>
-      <c r="BI1" s="57"/>
-      <c r="BJ1" s="58"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="49"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="49"/>
+      <c r="AR1" s="50"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="49"/>
+      <c r="AV1" s="50"/>
+      <c r="AW1" s="50"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="49"/>
+      <c r="AZ1" s="50"/>
+      <c r="BA1" s="50"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="49"/>
+      <c r="BD1" s="50"/>
+      <c r="BE1" s="50"/>
+      <c r="BF1" s="51"/>
+      <c r="BG1" s="49"/>
+      <c r="BH1" s="50"/>
+      <c r="BI1" s="50"/>
+      <c r="BJ1" s="51"/>
     </row>
     <row r="2" spans="1:63" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1169,140 +1185,63 @@
       <c r="Z2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="4"/>
+      <c r="BI2" s="4"/>
+      <c r="BJ2" s="7"/>
+    </row>
+    <row r="3" spans="1:63" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="52">
         <v>1</v>
       </c>
-      <c r="AD2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AW2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="BF2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="BH2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="BI2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="BJ2" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:63" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="76">
-        <v>1</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="46"/>
+      <c r="C3" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="56"/>
+      <c r="F3" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="N3" s="75"/>
       <c r="R3" s="11"/>
       <c r="S3" s="9"/>
       <c r="V3" s="11"/>
@@ -1328,21 +1267,17 @@
       <c r="BJ3" s="11"/>
     </row>
     <row r="4" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="18"/>
-      <c r="N4" s="48"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="N4" s="44"/>
       <c r="R4" s="14"/>
       <c r="S4" s="12"/>
       <c r="V4" s="14"/>
@@ -1368,25 +1303,22 @@
       <c r="BJ4" s="14"/>
     </row>
     <row r="5" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="50"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="40"/>
+      <c r="K5" s="76"/>
+      <c r="N5" s="44"/>
       <c r="R5" s="14"/>
-      <c r="S5" s="12"/>
-      <c r="V5" s="14"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="78"/>
       <c r="W5" s="12"/>
       <c r="Z5" s="14"/>
       <c r="AA5" s="12"/>
@@ -1409,22 +1341,22 @@
       <c r="BJ5" s="14"/>
     </row>
     <row r="6" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="53"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="77"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
@@ -1432,8 +1364,8 @@
       <c r="S6" s="12"/>
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="12"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="81"/>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
       <c r="Z6" s="14"/>
@@ -1475,19 +1407,19 @@
       <c r="BJ6" s="14"/>
     </row>
     <row r="7" spans="1:63" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="52">
         <v>2</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="25" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="26" t="s">
-        <v>24</v>
       </c>
       <c r="G7" s="9"/>
       <c r="J7" s="11"/>
@@ -1519,13 +1451,13 @@
       <c r="BJ7" s="11"/>
     </row>
     <row r="8" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="37" t="s">
-        <v>25</v>
+      <c r="A8" s="65"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="J8" s="14"/>
       <c r="N8" s="14"/>
@@ -1555,18 +1487,23 @@
       <c r="BJ8" s="14"/>
     </row>
     <row r="9" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="37" t="s">
-        <v>26</v>
+      <c r="A9" s="65"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="J9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="12"/>
-      <c r="R9" s="14"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="78"/>
       <c r="S9" s="12"/>
       <c r="V9" s="14"/>
       <c r="W9" s="12"/>
@@ -1591,29 +1528,29 @@
       <c r="BJ9" s="14"/>
     </row>
     <row r="10" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="27" t="s">
-        <v>27</v>
+      <c r="A10" s="65"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
       <c r="V10" s="14"/>
       <c r="W10" s="12"/>
       <c r="X10" s="13"/>
@@ -1657,17 +1594,17 @@
       <c r="BJ10" s="14"/>
     </row>
     <row r="11" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
-      <c r="B11" s="77">
+      <c r="A11" s="65"/>
+      <c r="B11" s="67">
         <v>3</v>
       </c>
-      <c r="C11" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="26" t="s">
-        <v>24</v>
+      <c r="C11" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="G11" s="9"/>
       <c r="J11" s="11"/>
@@ -1700,13 +1637,13 @@
       <c r="BK11" s="9"/>
     </row>
     <row r="12" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="37" t="s">
-        <v>25</v>
+      <c r="A12" s="65"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="G12" s="12"/>
       <c r="J12" s="14"/>
@@ -1738,13 +1675,13 @@
       <c r="BK12" s="12"/>
     </row>
     <row r="13" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="37" t="s">
-        <v>26</v>
+      <c r="A13" s="65"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="G13" s="12"/>
       <c r="J13" s="14"/>
@@ -1775,56 +1712,56 @@
       <c r="BJ13" s="14"/>
       <c r="BK13" s="12"/>
     </row>
-    <row r="14" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="38"/>
-      <c r="J14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="38"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="38"/>
-      <c r="V14" s="40"/>
-      <c r="W14" s="38"/>
-      <c r="Z14" s="40"/>
-      <c r="AA14" s="38"/>
-      <c r="AD14" s="40"/>
-      <c r="AE14" s="38"/>
-      <c r="AH14" s="40"/>
-      <c r="AI14" s="38"/>
-      <c r="AL14" s="40"/>
-      <c r="AM14" s="38"/>
-      <c r="AP14" s="40"/>
-      <c r="AQ14" s="38"/>
-      <c r="AT14" s="40"/>
-      <c r="AU14" s="38"/>
-      <c r="AX14" s="40"/>
-      <c r="AY14" s="38"/>
-      <c r="BB14" s="40"/>
-      <c r="BC14" s="38"/>
-      <c r="BF14" s="40"/>
-      <c r="BG14" s="38"/>
-      <c r="BJ14" s="40"/>
-      <c r="BK14" s="38"/>
+    <row r="14" spans="1:63" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="65"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="J14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="37"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="37"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="37"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="37"/>
+      <c r="AD14" s="39"/>
+      <c r="AE14" s="37"/>
+      <c r="AH14" s="39"/>
+      <c r="AI14" s="37"/>
+      <c r="AL14" s="39"/>
+      <c r="AM14" s="37"/>
+      <c r="AP14" s="39"/>
+      <c r="AQ14" s="37"/>
+      <c r="AT14" s="39"/>
+      <c r="AU14" s="37"/>
+      <c r="AX14" s="39"/>
+      <c r="AY14" s="37"/>
+      <c r="BB14" s="39"/>
+      <c r="BC14" s="37"/>
+      <c r="BF14" s="39"/>
+      <c r="BG14" s="37"/>
+      <c r="BJ14" s="39"/>
+      <c r="BK14" s="37"/>
     </row>
     <row r="15" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="76">
+      <c r="A15" s="65"/>
+      <c r="B15" s="73">
         <v>4</v>
       </c>
-      <c r="C15" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="37" t="s">
-        <v>24</v>
+      <c r="C15" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="36" t="s">
+        <v>22</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -1884,13 +1821,13 @@
       <c r="BJ15" s="14"/>
     </row>
     <row r="16" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="37" t="s">
-        <v>25</v>
+      <c r="A16" s="65"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1950,13 +1887,13 @@
       <c r="BJ16" s="14"/>
     </row>
     <row r="17" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="37" t="s">
-        <v>26</v>
+      <c r="A17" s="65"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -2016,13 +1953,13 @@
       <c r="BJ17" s="14"/>
     </row>
     <row r="18" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="27" t="s">
-        <v>27</v>
+      <c r="A18" s="65"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
@@ -2082,21 +2019,17 @@
       <c r="BJ18" s="14"/>
     </row>
     <row r="19" spans="1:62" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="76">
-        <v>5</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="26" t="s">
-        <v>24</v>
+      <c r="A19" s="65"/>
+      <c r="B19" s="52">
+        <v>2</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="G19" s="9"/>
       <c r="J19" s="11"/>
@@ -2128,13 +2061,13 @@
       <c r="BJ19" s="11"/>
     </row>
     <row r="20" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="37" t="s">
-        <v>25</v>
+      <c r="A20" s="65"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="J20" s="14"/>
       <c r="N20" s="14"/>
@@ -2164,13 +2097,13 @@
       <c r="BJ20" s="14"/>
     </row>
     <row r="21" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="76"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="37" t="s">
-        <v>26</v>
+      <c r="A21" s="65"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="J21" s="14"/>
       <c r="N21" s="14"/>
@@ -2200,13 +2133,13 @@
       <c r="BJ21" s="14"/>
     </row>
     <row r="22" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="27" t="s">
-        <v>27</v>
+      <c r="A22" s="65"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
@@ -2266,30 +2199,29 @@
       <c r="BJ22" s="14"/>
     </row>
     <row r="23" spans="1:62" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="76">
-        <v>6</v>
-      </c>
-      <c r="C23" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="26" t="s">
-        <v>24</v>
+      <c r="A23" s="65"/>
+      <c r="B23" s="67">
+        <v>3</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="G23" s="9"/>
       <c r="J23" s="11"/>
       <c r="K23" s="9"/>
-      <c r="O23" s="45"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="9"/>
       <c r="R23" s="11"/>
-      <c r="S23" s="45"/>
+      <c r="S23" s="9"/>
       <c r="V23" s="11"/>
       <c r="W23" s="9"/>
       <c r="Z23" s="11"/>
-      <c r="AA23" s="45"/>
+      <c r="AA23" s="9"/>
       <c r="AD23" s="11"/>
       <c r="AE23" s="9"/>
       <c r="AH23" s="11"/>
@@ -2309,14 +2241,15 @@
       <c r="BJ23" s="11"/>
     </row>
     <row r="24" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="37" t="s">
-        <v>25</v>
-      </c>
+      <c r="A24" s="65"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="12"/>
       <c r="J24" s="14"/>
       <c r="N24" s="14"/>
       <c r="O24" s="12"/>
@@ -2345,20 +2278,22 @@
       <c r="BJ24" s="14"/>
     </row>
     <row r="25" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="37" t="s">
-        <v>26</v>
-      </c>
+      <c r="A25" s="65"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="12"/>
       <c r="J25" s="14"/>
       <c r="N25" s="14"/>
       <c r="O25" s="12"/>
-      <c r="S25" s="49"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="12"/>
       <c r="V25" s="14"/>
-      <c r="W25" s="49"/>
+      <c r="W25" s="12"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="12"/>
       <c r="AD25" s="14"/>
@@ -2380,236 +2315,2114 @@
       <c r="BJ25" s="14"/>
     </row>
     <row r="26" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="74"/>
-      <c r="B26" s="76"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="12"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="13"/>
-      <c r="AD26" s="14"/>
-      <c r="AE26" s="12"/>
-      <c r="AF26" s="13"/>
-      <c r="AG26" s="13"/>
-      <c r="AH26" s="14"/>
-      <c r="AI26" s="12"/>
-      <c r="AJ26" s="13"/>
-      <c r="AK26" s="13"/>
-      <c r="AL26" s="14"/>
-      <c r="AM26" s="12"/>
-      <c r="AN26" s="13"/>
-      <c r="AO26" s="13"/>
-      <c r="AP26" s="14"/>
-      <c r="AQ26" s="12"/>
-      <c r="AR26" s="13"/>
-      <c r="AS26" s="13"/>
-      <c r="AT26" s="14"/>
-      <c r="AU26" s="12"/>
-      <c r="AV26" s="13"/>
-      <c r="AW26" s="13"/>
-      <c r="AX26" s="14"/>
-      <c r="AY26" s="12"/>
-      <c r="AZ26" s="13"/>
-      <c r="BA26" s="13"/>
-      <c r="BB26" s="14"/>
-      <c r="BC26" s="12"/>
-      <c r="BD26" s="13"/>
-      <c r="BE26" s="13"/>
-      <c r="BF26" s="14"/>
-      <c r="BG26" s="12"/>
-      <c r="BH26" s="13"/>
-      <c r="BI26" s="13"/>
-      <c r="BJ26" s="14"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="39"/>
+      <c r="AA26" s="37"/>
+      <c r="AB26" s="38"/>
+      <c r="AC26" s="38"/>
+      <c r="AD26" s="39"/>
+      <c r="AE26" s="37"/>
+      <c r="AF26" s="38"/>
+      <c r="AG26" s="38"/>
+      <c r="AH26" s="39"/>
+      <c r="AI26" s="37"/>
+      <c r="AJ26" s="38"/>
+      <c r="AK26" s="38"/>
+      <c r="AL26" s="39"/>
+      <c r="AM26" s="37"/>
+      <c r="AN26" s="38"/>
+      <c r="AO26" s="38"/>
+      <c r="AP26" s="39"/>
+      <c r="AQ26" s="37"/>
+      <c r="AR26" s="38"/>
+      <c r="AS26" s="38"/>
+      <c r="AT26" s="39"/>
+      <c r="AU26" s="37"/>
+      <c r="AV26" s="38"/>
+      <c r="AW26" s="38"/>
+      <c r="AX26" s="39"/>
+      <c r="AY26" s="37"/>
+      <c r="AZ26" s="38"/>
+      <c r="BA26" s="38"/>
+      <c r="BB26" s="39"/>
+      <c r="BC26" s="37"/>
+      <c r="BD26" s="38"/>
+      <c r="BE26" s="38"/>
+      <c r="BF26" s="39"/>
+      <c r="BG26" s="37"/>
+      <c r="BH26" s="38"/>
+      <c r="BI26" s="38"/>
+      <c r="BJ26" s="39"/>
     </row>
     <row r="27" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="55">
+      <c r="A27" s="65"/>
+      <c r="B27" s="73">
+        <v>4</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="13"/>
+      <c r="AC27" s="13"/>
+      <c r="AD27" s="14"/>
+      <c r="AE27" s="12"/>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="13"/>
+      <c r="AH27" s="14"/>
+      <c r="AI27" s="12"/>
+      <c r="AJ27" s="13"/>
+      <c r="AK27" s="13"/>
+      <c r="AL27" s="14"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="13"/>
+      <c r="AO27" s="13"/>
+      <c r="AP27" s="14"/>
+      <c r="AQ27" s="12"/>
+      <c r="AR27" s="13"/>
+      <c r="AS27" s="13"/>
+      <c r="AT27" s="14"/>
+      <c r="AU27" s="12"/>
+      <c r="AV27" s="13"/>
+      <c r="AW27" s="13"/>
+      <c r="AX27" s="14"/>
+      <c r="AY27" s="12"/>
+      <c r="AZ27" s="13"/>
+      <c r="BA27" s="13"/>
+      <c r="BB27" s="14"/>
+      <c r="BC27" s="12"/>
+      <c r="BD27" s="13"/>
+      <c r="BE27" s="13"/>
+      <c r="BF27" s="14"/>
+      <c r="BG27" s="12"/>
+      <c r="BH27" s="13"/>
+      <c r="BI27" s="13"/>
+      <c r="BJ27" s="14"/>
+    </row>
+    <row r="28" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="65"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="13"/>
+      <c r="AC28" s="13"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="13"/>
+      <c r="AH28" s="14"/>
+      <c r="AI28" s="12"/>
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="13"/>
+      <c r="AL28" s="14"/>
+      <c r="AM28" s="12"/>
+      <c r="AN28" s="13"/>
+      <c r="AO28" s="13"/>
+      <c r="AP28" s="14"/>
+      <c r="AQ28" s="12"/>
+      <c r="AR28" s="13"/>
+      <c r="AS28" s="13"/>
+      <c r="AT28" s="14"/>
+      <c r="AU28" s="12"/>
+      <c r="AV28" s="13"/>
+      <c r="AW28" s="13"/>
+      <c r="AX28" s="14"/>
+      <c r="AY28" s="12"/>
+      <c r="AZ28" s="13"/>
+      <c r="BA28" s="13"/>
+      <c r="BB28" s="14"/>
+      <c r="BC28" s="12"/>
+      <c r="BD28" s="13"/>
+      <c r="BE28" s="13"/>
+      <c r="BF28" s="14"/>
+      <c r="BG28" s="12"/>
+      <c r="BH28" s="13"/>
+      <c r="BI28" s="13"/>
+      <c r="BJ28" s="14"/>
+    </row>
+    <row r="29" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A29" s="65"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="13"/>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="14"/>
+      <c r="AE29" s="12"/>
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="13"/>
+      <c r="AH29" s="14"/>
+      <c r="AI29" s="12"/>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="13"/>
+      <c r="AL29" s="14"/>
+      <c r="AM29" s="12"/>
+      <c r="AN29" s="13"/>
+      <c r="AO29" s="13"/>
+      <c r="AP29" s="14"/>
+      <c r="AQ29" s="12"/>
+      <c r="AR29" s="13"/>
+      <c r="AS29" s="13"/>
+      <c r="AT29" s="14"/>
+      <c r="AU29" s="12"/>
+      <c r="AV29" s="13"/>
+      <c r="AW29" s="13"/>
+      <c r="AX29" s="14"/>
+      <c r="AY29" s="12"/>
+      <c r="AZ29" s="13"/>
+      <c r="BA29" s="13"/>
+      <c r="BB29" s="14"/>
+      <c r="BC29" s="12"/>
+      <c r="BD29" s="13"/>
+      <c r="BE29" s="13"/>
+      <c r="BF29" s="14"/>
+      <c r="BG29" s="12"/>
+      <c r="BH29" s="13"/>
+      <c r="BI29" s="13"/>
+      <c r="BJ29" s="14"/>
+    </row>
+    <row r="30" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A30" s="65"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="13"/>
+      <c r="AC30" s="13"/>
+      <c r="AD30" s="14"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="13"/>
+      <c r="AH30" s="14"/>
+      <c r="AI30" s="12"/>
+      <c r="AJ30" s="13"/>
+      <c r="AK30" s="13"/>
+      <c r="AL30" s="14"/>
+      <c r="AM30" s="12"/>
+      <c r="AN30" s="13"/>
+      <c r="AO30" s="13"/>
+      <c r="AP30" s="14"/>
+      <c r="AQ30" s="12"/>
+      <c r="AR30" s="13"/>
+      <c r="AS30" s="13"/>
+      <c r="AT30" s="14"/>
+      <c r="AU30" s="12"/>
+      <c r="AV30" s="13"/>
+      <c r="AW30" s="13"/>
+      <c r="AX30" s="14"/>
+      <c r="AY30" s="12"/>
+      <c r="AZ30" s="13"/>
+      <c r="BA30" s="13"/>
+      <c r="BB30" s="14"/>
+      <c r="BC30" s="12"/>
+      <c r="BD30" s="13"/>
+      <c r="BE30" s="13"/>
+      <c r="BF30" s="14"/>
+      <c r="BG30" s="12"/>
+      <c r="BH30" s="13"/>
+      <c r="BI30" s="13"/>
+      <c r="BJ30" s="14"/>
+    </row>
+    <row r="31" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="65"/>
+      <c r="B31" s="52">
+        <v>2</v>
+      </c>
+      <c r="C31" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="56"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="10"/>
+      <c r="AK31" s="10"/>
+      <c r="AL31" s="11"/>
+      <c r="AM31" s="9"/>
+      <c r="AN31" s="10"/>
+      <c r="AO31" s="10"/>
+      <c r="AP31" s="11"/>
+      <c r="AQ31" s="9"/>
+      <c r="AR31" s="10"/>
+      <c r="AS31" s="10"/>
+      <c r="AT31" s="11"/>
+      <c r="AU31" s="9"/>
+      <c r="AV31" s="10"/>
+      <c r="AW31" s="10"/>
+      <c r="AX31" s="11"/>
+      <c r="AY31" s="9"/>
+      <c r="AZ31" s="10"/>
+      <c r="BA31" s="10"/>
+      <c r="BB31" s="11"/>
+      <c r="BC31" s="9"/>
+      <c r="BD31" s="10"/>
+      <c r="BE31" s="10"/>
+      <c r="BF31" s="11"/>
+      <c r="BG31" s="9"/>
+      <c r="BH31" s="10"/>
+      <c r="BI31" s="10"/>
+      <c r="BJ31" s="11"/>
+    </row>
+    <row r="32" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A32" s="65"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="13"/>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="14"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="13"/>
+      <c r="AG32" s="13"/>
+      <c r="AH32" s="14"/>
+      <c r="AI32" s="12"/>
+      <c r="AJ32" s="13"/>
+      <c r="AK32" s="13"/>
+      <c r="AL32" s="14"/>
+      <c r="AM32" s="12"/>
+      <c r="AN32" s="13"/>
+      <c r="AO32" s="13"/>
+      <c r="AP32" s="14"/>
+      <c r="AQ32" s="12"/>
+      <c r="AR32" s="13"/>
+      <c r="AS32" s="13"/>
+      <c r="AT32" s="14"/>
+      <c r="AU32" s="12"/>
+      <c r="AV32" s="13"/>
+      <c r="AW32" s="13"/>
+      <c r="AX32" s="14"/>
+      <c r="AY32" s="12"/>
+      <c r="AZ32" s="13"/>
+      <c r="BA32" s="13"/>
+      <c r="BB32" s="14"/>
+      <c r="BC32" s="12"/>
+      <c r="BD32" s="13"/>
+      <c r="BE32" s="13"/>
+      <c r="BF32" s="14"/>
+      <c r="BG32" s="12"/>
+      <c r="BH32" s="13"/>
+      <c r="BI32" s="13"/>
+      <c r="BJ32" s="14"/>
+    </row>
+    <row r="33" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A33" s="65"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="78"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="13"/>
+      <c r="AC33" s="13"/>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="13"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="12"/>
+      <c r="AJ33" s="13"/>
+      <c r="AK33" s="13"/>
+      <c r="AL33" s="14"/>
+      <c r="AM33" s="12"/>
+      <c r="AN33" s="13"/>
+      <c r="AO33" s="13"/>
+      <c r="AP33" s="14"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="13"/>
+      <c r="AS33" s="13"/>
+      <c r="AT33" s="14"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="13"/>
+      <c r="AW33" s="13"/>
+      <c r="AX33" s="14"/>
+      <c r="AY33" s="12"/>
+      <c r="AZ33" s="13"/>
+      <c r="BA33" s="13"/>
+      <c r="BB33" s="14"/>
+      <c r="BC33" s="12"/>
+      <c r="BD33" s="13"/>
+      <c r="BE33" s="13"/>
+      <c r="BF33" s="14"/>
+      <c r="BG33" s="12"/>
+      <c r="BH33" s="13"/>
+      <c r="BI33" s="13"/>
+      <c r="BJ33" s="14"/>
+    </row>
+    <row r="34" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A34" s="65"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="80"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="80"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="13"/>
+      <c r="AC34" s="13"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="13"/>
+      <c r="AG34" s="13"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="12"/>
+      <c r="AJ34" s="13"/>
+      <c r="AK34" s="13"/>
+      <c r="AL34" s="14"/>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="13"/>
+      <c r="AO34" s="13"/>
+      <c r="AP34" s="14"/>
+      <c r="AQ34" s="12"/>
+      <c r="AR34" s="13"/>
+      <c r="AS34" s="13"/>
+      <c r="AT34" s="14"/>
+      <c r="AU34" s="12"/>
+      <c r="AV34" s="13"/>
+      <c r="AW34" s="13"/>
+      <c r="AX34" s="14"/>
+      <c r="AY34" s="12"/>
+      <c r="AZ34" s="13"/>
+      <c r="BA34" s="13"/>
+      <c r="BB34" s="14"/>
+      <c r="BC34" s="12"/>
+      <c r="BD34" s="13"/>
+      <c r="BE34" s="13"/>
+      <c r="BF34" s="14"/>
+      <c r="BG34" s="12"/>
+      <c r="BH34" s="13"/>
+      <c r="BI34" s="13"/>
+      <c r="BJ34" s="14"/>
+    </row>
+    <row r="35" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A35" s="65"/>
+      <c r="B35" s="67">
+        <v>3</v>
+      </c>
+      <c r="C35" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="56"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="9"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="10"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="9"/>
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="10"/>
+      <c r="AH35" s="11"/>
+      <c r="AI35" s="9"/>
+      <c r="AJ35" s="10"/>
+      <c r="AK35" s="10"/>
+      <c r="AL35" s="11"/>
+      <c r="AM35" s="9"/>
+      <c r="AN35" s="10"/>
+      <c r="AO35" s="10"/>
+      <c r="AP35" s="11"/>
+      <c r="AQ35" s="9"/>
+      <c r="AR35" s="10"/>
+      <c r="AS35" s="10"/>
+      <c r="AT35" s="11"/>
+      <c r="AU35" s="9"/>
+      <c r="AV35" s="10"/>
+      <c r="AW35" s="10"/>
+      <c r="AX35" s="11"/>
+      <c r="AY35" s="9"/>
+      <c r="AZ35" s="10"/>
+      <c r="BA35" s="10"/>
+      <c r="BB35" s="11"/>
+      <c r="BC35" s="9"/>
+      <c r="BD35" s="10"/>
+      <c r="BE35" s="10"/>
+      <c r="BF35" s="11"/>
+      <c r="BG35" s="9"/>
+      <c r="BH35" s="10"/>
+      <c r="BI35" s="10"/>
+      <c r="BJ35" s="11"/>
+    </row>
+    <row r="36" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A36" s="65"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="13"/>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="13"/>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="12"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="13"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="12"/>
+      <c r="AN36" s="13"/>
+      <c r="AO36" s="13"/>
+      <c r="AP36" s="14"/>
+      <c r="AQ36" s="12"/>
+      <c r="AR36" s="13"/>
+      <c r="AS36" s="13"/>
+      <c r="AT36" s="14"/>
+      <c r="AU36" s="12"/>
+      <c r="AV36" s="13"/>
+      <c r="AW36" s="13"/>
+      <c r="AX36" s="14"/>
+      <c r="AY36" s="12"/>
+      <c r="AZ36" s="13"/>
+      <c r="BA36" s="13"/>
+      <c r="BB36" s="14"/>
+      <c r="BC36" s="12"/>
+      <c r="BD36" s="13"/>
+      <c r="BE36" s="13"/>
+      <c r="BF36" s="14"/>
+      <c r="BG36" s="12"/>
+      <c r="BH36" s="13"/>
+      <c r="BI36" s="13"/>
+      <c r="BJ36" s="14"/>
+    </row>
+    <row r="37" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A37" s="65"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="12"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="12"/>
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="12"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="12"/>
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="13"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="12"/>
+      <c r="AN37" s="13"/>
+      <c r="AO37" s="13"/>
+      <c r="AP37" s="14"/>
+      <c r="AQ37" s="12"/>
+      <c r="AR37" s="13"/>
+      <c r="AS37" s="13"/>
+      <c r="AT37" s="14"/>
+      <c r="AU37" s="12"/>
+      <c r="AV37" s="13"/>
+      <c r="AW37" s="13"/>
+      <c r="AX37" s="14"/>
+      <c r="AY37" s="12"/>
+      <c r="AZ37" s="13"/>
+      <c r="BA37" s="13"/>
+      <c r="BB37" s="14"/>
+      <c r="BC37" s="12"/>
+      <c r="BD37" s="13"/>
+      <c r="BE37" s="13"/>
+      <c r="BF37" s="14"/>
+      <c r="BG37" s="12"/>
+      <c r="BH37" s="13"/>
+      <c r="BI37" s="13"/>
+      <c r="BJ37" s="14"/>
+    </row>
+    <row r="38" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A38" s="65"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="37"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="38"/>
+      <c r="R38" s="39"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="38"/>
+      <c r="U38" s="38"/>
+      <c r="V38" s="39"/>
+      <c r="W38" s="37"/>
+      <c r="X38" s="38"/>
+      <c r="Y38" s="38"/>
+      <c r="Z38" s="39"/>
+      <c r="AA38" s="37"/>
+      <c r="AB38" s="38"/>
+      <c r="AC38" s="38"/>
+      <c r="AD38" s="39"/>
+      <c r="AE38" s="37"/>
+      <c r="AF38" s="38"/>
+      <c r="AG38" s="38"/>
+      <c r="AH38" s="39"/>
+      <c r="AI38" s="37"/>
+      <c r="AJ38" s="38"/>
+      <c r="AK38" s="38"/>
+      <c r="AL38" s="39"/>
+      <c r="AM38" s="37"/>
+      <c r="AN38" s="38"/>
+      <c r="AO38" s="38"/>
+      <c r="AP38" s="39"/>
+      <c r="AQ38" s="37"/>
+      <c r="AR38" s="38"/>
+      <c r="AS38" s="38"/>
+      <c r="AT38" s="39"/>
+      <c r="AU38" s="37"/>
+      <c r="AV38" s="38"/>
+      <c r="AW38" s="38"/>
+      <c r="AX38" s="39"/>
+      <c r="AY38" s="37"/>
+      <c r="AZ38" s="38"/>
+      <c r="BA38" s="38"/>
+      <c r="BB38" s="39"/>
+      <c r="BC38" s="37"/>
+      <c r="BD38" s="38"/>
+      <c r="BE38" s="38"/>
+      <c r="BF38" s="39"/>
+      <c r="BG38" s="37"/>
+      <c r="BH38" s="38"/>
+      <c r="BI38" s="38"/>
+      <c r="BJ38" s="39"/>
+    </row>
+    <row r="39" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A39" s="65"/>
+      <c r="B39" s="73">
+        <v>4</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="56"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="12"/>
+      <c r="X39" s="13"/>
+      <c r="Y39" s="13"/>
+      <c r="Z39" s="14"/>
+      <c r="AA39" s="12"/>
+      <c r="AB39" s="13"/>
+      <c r="AC39" s="13"/>
+      <c r="AD39" s="14"/>
+      <c r="AE39" s="12"/>
+      <c r="AF39" s="13"/>
+      <c r="AG39" s="13"/>
+      <c r="AH39" s="14"/>
+      <c r="AI39" s="12"/>
+      <c r="AJ39" s="13"/>
+      <c r="AK39" s="13"/>
+      <c r="AL39" s="14"/>
+      <c r="AM39" s="12"/>
+      <c r="AN39" s="13"/>
+      <c r="AO39" s="13"/>
+      <c r="AP39" s="14"/>
+      <c r="AQ39" s="12"/>
+      <c r="AR39" s="13"/>
+      <c r="AS39" s="13"/>
+      <c r="AT39" s="14"/>
+      <c r="AU39" s="12"/>
+      <c r="AV39" s="13"/>
+      <c r="AW39" s="13"/>
+      <c r="AX39" s="14"/>
+      <c r="AY39" s="12"/>
+      <c r="AZ39" s="13"/>
+      <c r="BA39" s="13"/>
+      <c r="BB39" s="14"/>
+      <c r="BC39" s="12"/>
+      <c r="BD39" s="13"/>
+      <c r="BE39" s="13"/>
+      <c r="BF39" s="14"/>
+      <c r="BG39" s="12"/>
+      <c r="BH39" s="13"/>
+      <c r="BI39" s="13"/>
+      <c r="BJ39" s="14"/>
+    </row>
+    <row r="40" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A40" s="65"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="12"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="12"/>
+      <c r="X40" s="13"/>
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="12"/>
+      <c r="AB40" s="13"/>
+      <c r="AC40" s="13"/>
+      <c r="AD40" s="14"/>
+      <c r="AE40" s="12"/>
+      <c r="AF40" s="13"/>
+      <c r="AG40" s="13"/>
+      <c r="AH40" s="14"/>
+      <c r="AI40" s="12"/>
+      <c r="AJ40" s="13"/>
+      <c r="AK40" s="13"/>
+      <c r="AL40" s="14"/>
+      <c r="AM40" s="12"/>
+      <c r="AN40" s="13"/>
+      <c r="AO40" s="13"/>
+      <c r="AP40" s="14"/>
+      <c r="AQ40" s="12"/>
+      <c r="AR40" s="13"/>
+      <c r="AS40" s="13"/>
+      <c r="AT40" s="14"/>
+      <c r="AU40" s="12"/>
+      <c r="AV40" s="13"/>
+      <c r="AW40" s="13"/>
+      <c r="AX40" s="14"/>
+      <c r="AY40" s="12"/>
+      <c r="AZ40" s="13"/>
+      <c r="BA40" s="13"/>
+      <c r="BB40" s="14"/>
+      <c r="BC40" s="12"/>
+      <c r="BD40" s="13"/>
+      <c r="BE40" s="13"/>
+      <c r="BF40" s="14"/>
+      <c r="BG40" s="12"/>
+      <c r="BH40" s="13"/>
+      <c r="BI40" s="13"/>
+      <c r="BJ40" s="14"/>
+    </row>
+    <row r="41" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A41" s="65"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="14"/>
+      <c r="AA41" s="12"/>
+      <c r="AB41" s="13"/>
+      <c r="AC41" s="13"/>
+      <c r="AD41" s="14"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="13"/>
+      <c r="AG41" s="13"/>
+      <c r="AH41" s="14"/>
+      <c r="AI41" s="12"/>
+      <c r="AJ41" s="13"/>
+      <c r="AK41" s="13"/>
+      <c r="AL41" s="14"/>
+      <c r="AM41" s="12"/>
+      <c r="AN41" s="13"/>
+      <c r="AO41" s="13"/>
+      <c r="AP41" s="14"/>
+      <c r="AQ41" s="12"/>
+      <c r="AR41" s="13"/>
+      <c r="AS41" s="13"/>
+      <c r="AT41" s="14"/>
+      <c r="AU41" s="12"/>
+      <c r="AV41" s="13"/>
+      <c r="AW41" s="13"/>
+      <c r="AX41" s="14"/>
+      <c r="AY41" s="12"/>
+      <c r="AZ41" s="13"/>
+      <c r="BA41" s="13"/>
+      <c r="BB41" s="14"/>
+      <c r="BC41" s="12"/>
+      <c r="BD41" s="13"/>
+      <c r="BE41" s="13"/>
+      <c r="BF41" s="14"/>
+      <c r="BG41" s="12"/>
+      <c r="BH41" s="13"/>
+      <c r="BI41" s="13"/>
+      <c r="BJ41" s="14"/>
+    </row>
+    <row r="42" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A42" s="65"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="12"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="14"/>
+      <c r="AE42" s="12"/>
+      <c r="AF42" s="13"/>
+      <c r="AG42" s="13"/>
+      <c r="AH42" s="14"/>
+      <c r="AI42" s="12"/>
+      <c r="AJ42" s="13"/>
+      <c r="AK42" s="13"/>
+      <c r="AL42" s="14"/>
+      <c r="AM42" s="12"/>
+      <c r="AN42" s="13"/>
+      <c r="AO42" s="13"/>
+      <c r="AP42" s="14"/>
+      <c r="AQ42" s="12"/>
+      <c r="AR42" s="13"/>
+      <c r="AS42" s="13"/>
+      <c r="AT42" s="14"/>
+      <c r="AU42" s="12"/>
+      <c r="AV42" s="13"/>
+      <c r="AW42" s="13"/>
+      <c r="AX42" s="14"/>
+      <c r="AY42" s="12"/>
+      <c r="AZ42" s="13"/>
+      <c r="BA42" s="13"/>
+      <c r="BB42" s="14"/>
+      <c r="BC42" s="12"/>
+      <c r="BD42" s="13"/>
+      <c r="BE42" s="13"/>
+      <c r="BF42" s="14"/>
+      <c r="BG42" s="12"/>
+      <c r="BH42" s="13"/>
+      <c r="BI42" s="13"/>
+      <c r="BJ42" s="14"/>
+    </row>
+    <row r="43" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="65"/>
+      <c r="B43" s="52">
+        <v>2</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="9"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="9"/>
+      <c r="AB43" s="10"/>
+      <c r="AC43" s="10"/>
+      <c r="AD43" s="11"/>
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="10"/>
+      <c r="AG43" s="10"/>
+      <c r="AH43" s="11"/>
+      <c r="AI43" s="9"/>
+      <c r="AJ43" s="10"/>
+      <c r="AK43" s="10"/>
+      <c r="AL43" s="11"/>
+      <c r="AM43" s="9"/>
+      <c r="AN43" s="10"/>
+      <c r="AO43" s="10"/>
+      <c r="AP43" s="11"/>
+      <c r="AQ43" s="9"/>
+      <c r="AR43" s="10"/>
+      <c r="AS43" s="10"/>
+      <c r="AT43" s="11"/>
+      <c r="AU43" s="9"/>
+      <c r="AV43" s="10"/>
+      <c r="AW43" s="10"/>
+      <c r="AX43" s="11"/>
+      <c r="AY43" s="9"/>
+      <c r="AZ43" s="10"/>
+      <c r="BA43" s="10"/>
+      <c r="BB43" s="11"/>
+      <c r="BC43" s="9"/>
+      <c r="BD43" s="10"/>
+      <c r="BE43" s="10"/>
+      <c r="BF43" s="11"/>
+      <c r="BG43" s="9"/>
+      <c r="BH43" s="10"/>
+      <c r="BI43" s="10"/>
+      <c r="BJ43" s="11"/>
+    </row>
+    <row r="44" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A44" s="65"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="13"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="14"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="13"/>
+      <c r="AC44" s="13"/>
+      <c r="AD44" s="14"/>
+      <c r="AE44" s="12"/>
+      <c r="AF44" s="13"/>
+      <c r="AG44" s="13"/>
+      <c r="AH44" s="14"/>
+      <c r="AI44" s="12"/>
+      <c r="AJ44" s="13"/>
+      <c r="AK44" s="13"/>
+      <c r="AL44" s="14"/>
+      <c r="AM44" s="12"/>
+      <c r="AN44" s="13"/>
+      <c r="AO44" s="13"/>
+      <c r="AP44" s="14"/>
+      <c r="AQ44" s="12"/>
+      <c r="AR44" s="13"/>
+      <c r="AS44" s="13"/>
+      <c r="AT44" s="14"/>
+      <c r="AU44" s="12"/>
+      <c r="AV44" s="13"/>
+      <c r="AW44" s="13"/>
+      <c r="AX44" s="14"/>
+      <c r="AY44" s="12"/>
+      <c r="AZ44" s="13"/>
+      <c r="BA44" s="13"/>
+      <c r="BB44" s="14"/>
+      <c r="BC44" s="12"/>
+      <c r="BD44" s="13"/>
+      <c r="BE44" s="13"/>
+      <c r="BF44" s="14"/>
+      <c r="BG44" s="12"/>
+      <c r="BH44" s="13"/>
+      <c r="BI44" s="13"/>
+      <c r="BJ44" s="14"/>
+    </row>
+    <row r="45" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A45" s="65"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="14"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="13"/>
+      <c r="AC45" s="13"/>
+      <c r="AD45" s="14"/>
+      <c r="AE45" s="12"/>
+      <c r="AF45" s="13"/>
+      <c r="AG45" s="13"/>
+      <c r="AH45" s="14"/>
+      <c r="AI45" s="12"/>
+      <c r="AJ45" s="13"/>
+      <c r="AK45" s="13"/>
+      <c r="AL45" s="14"/>
+      <c r="AM45" s="12"/>
+      <c r="AN45" s="13"/>
+      <c r="AO45" s="13"/>
+      <c r="AP45" s="14"/>
+      <c r="AQ45" s="12"/>
+      <c r="AR45" s="13"/>
+      <c r="AS45" s="13"/>
+      <c r="AT45" s="14"/>
+      <c r="AU45" s="12"/>
+      <c r="AV45" s="13"/>
+      <c r="AW45" s="13"/>
+      <c r="AX45" s="14"/>
+      <c r="AY45" s="12"/>
+      <c r="AZ45" s="13"/>
+      <c r="BA45" s="13"/>
+      <c r="BB45" s="14"/>
+      <c r="BC45" s="12"/>
+      <c r="BD45" s="13"/>
+      <c r="BE45" s="13"/>
+      <c r="BF45" s="14"/>
+      <c r="BG45" s="12"/>
+      <c r="BH45" s="13"/>
+      <c r="BI45" s="13"/>
+      <c r="BJ45" s="14"/>
+    </row>
+    <row r="46" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A46" s="65"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="13"/>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="14"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="13"/>
+      <c r="AD46" s="14"/>
+      <c r="AE46" s="12"/>
+      <c r="AF46" s="13"/>
+      <c r="AG46" s="13"/>
+      <c r="AH46" s="14"/>
+      <c r="AI46" s="12"/>
+      <c r="AJ46" s="13"/>
+      <c r="AK46" s="13"/>
+      <c r="AL46" s="14"/>
+      <c r="AM46" s="12"/>
+      <c r="AN46" s="13"/>
+      <c r="AO46" s="13"/>
+      <c r="AP46" s="14"/>
+      <c r="AQ46" s="12"/>
+      <c r="AR46" s="13"/>
+      <c r="AS46" s="13"/>
+      <c r="AT46" s="14"/>
+      <c r="AU46" s="12"/>
+      <c r="AV46" s="13"/>
+      <c r="AW46" s="13"/>
+      <c r="AX46" s="14"/>
+      <c r="AY46" s="12"/>
+      <c r="AZ46" s="13"/>
+      <c r="BA46" s="13"/>
+      <c r="BB46" s="14"/>
+      <c r="BC46" s="12"/>
+      <c r="BD46" s="13"/>
+      <c r="BE46" s="13"/>
+      <c r="BF46" s="14"/>
+      <c r="BG46" s="12"/>
+      <c r="BH46" s="13"/>
+      <c r="BI46" s="13"/>
+      <c r="BJ46" s="14"/>
+    </row>
+    <row r="47" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A47" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="52">
+        <v>5</v>
+      </c>
+      <c r="C47" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="57"/>
+      <c r="F47" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="11"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="10"/>
+      <c r="AC47" s="10"/>
+      <c r="AD47" s="11"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="10"/>
+      <c r="AG47" s="10"/>
+      <c r="AH47" s="11"/>
+      <c r="AI47" s="9"/>
+      <c r="AJ47" s="10"/>
+      <c r="AK47" s="10"/>
+      <c r="AL47" s="11"/>
+      <c r="AM47" s="9"/>
+      <c r="AN47" s="10"/>
+      <c r="AO47" s="10"/>
+      <c r="AP47" s="11"/>
+      <c r="AQ47" s="9"/>
+      <c r="AR47" s="10"/>
+      <c r="AS47" s="10"/>
+      <c r="AT47" s="11"/>
+      <c r="AU47" s="9"/>
+      <c r="AV47" s="10"/>
+      <c r="AW47" s="10"/>
+      <c r="AX47" s="11"/>
+      <c r="AY47" s="9"/>
+      <c r="AZ47" s="10"/>
+      <c r="BA47" s="10"/>
+      <c r="BB47" s="11"/>
+      <c r="BC47" s="9"/>
+      <c r="BD47" s="10"/>
+      <c r="BE47" s="10"/>
+      <c r="BF47" s="11"/>
+      <c r="BG47" s="9"/>
+      <c r="BH47" s="10"/>
+      <c r="BI47" s="10"/>
+      <c r="BJ47" s="11"/>
+    </row>
+    <row r="48" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A48" s="65"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="12"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="12"/>
+      <c r="X48" s="13"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="14"/>
+      <c r="AA48" s="12"/>
+      <c r="AB48" s="13"/>
+      <c r="AC48" s="13"/>
+      <c r="AD48" s="14"/>
+      <c r="AE48" s="12"/>
+      <c r="AF48" s="13"/>
+      <c r="AG48" s="13"/>
+      <c r="AH48" s="14"/>
+      <c r="AI48" s="12"/>
+      <c r="AJ48" s="13"/>
+      <c r="AK48" s="13"/>
+      <c r="AL48" s="14"/>
+      <c r="AM48" s="12"/>
+      <c r="AN48" s="13"/>
+      <c r="AO48" s="13"/>
+      <c r="AP48" s="14"/>
+      <c r="AQ48" s="12"/>
+      <c r="AR48" s="13"/>
+      <c r="AS48" s="13"/>
+      <c r="AT48" s="14"/>
+      <c r="AU48" s="12"/>
+      <c r="AV48" s="13"/>
+      <c r="AW48" s="13"/>
+      <c r="AX48" s="14"/>
+      <c r="AY48" s="12"/>
+      <c r="AZ48" s="13"/>
+      <c r="BA48" s="13"/>
+      <c r="BB48" s="14"/>
+      <c r="BC48" s="12"/>
+      <c r="BD48" s="13"/>
+      <c r="BE48" s="13"/>
+      <c r="BF48" s="14"/>
+      <c r="BG48" s="12"/>
+      <c r="BH48" s="13"/>
+      <c r="BI48" s="13"/>
+      <c r="BJ48" s="14"/>
+    </row>
+    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A49" s="65"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="12"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="14"/>
+      <c r="AA49" s="12"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="13"/>
+      <c r="AD49" s="14"/>
+      <c r="AE49" s="12"/>
+      <c r="AF49" s="13"/>
+      <c r="AG49" s="13"/>
+      <c r="AH49" s="14"/>
+      <c r="AI49" s="12"/>
+      <c r="AJ49" s="13"/>
+      <c r="AK49" s="13"/>
+      <c r="AL49" s="14"/>
+      <c r="AM49" s="12"/>
+      <c r="AN49" s="13"/>
+      <c r="AO49" s="13"/>
+      <c r="AP49" s="14"/>
+      <c r="AQ49" s="12"/>
+      <c r="AR49" s="13"/>
+      <c r="AS49" s="13"/>
+      <c r="AT49" s="14"/>
+      <c r="AU49" s="12"/>
+      <c r="AV49" s="13"/>
+      <c r="AW49" s="13"/>
+      <c r="AX49" s="14"/>
+      <c r="AY49" s="12"/>
+      <c r="AZ49" s="13"/>
+      <c r="BA49" s="13"/>
+      <c r="BB49" s="14"/>
+      <c r="BC49" s="12"/>
+      <c r="BD49" s="13"/>
+      <c r="BE49" s="13"/>
+      <c r="BF49" s="14"/>
+      <c r="BG49" s="12"/>
+      <c r="BH49" s="13"/>
+      <c r="BI49" s="13"/>
+      <c r="BJ49" s="14"/>
+    </row>
+    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A50" s="66"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="12"/>
+      <c r="X50" s="13"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="14"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="13"/>
+      <c r="AC50" s="13"/>
+      <c r="AD50" s="14"/>
+      <c r="AE50" s="12"/>
+      <c r="AF50" s="13"/>
+      <c r="AG50" s="13"/>
+      <c r="AH50" s="14"/>
+      <c r="AI50" s="12"/>
+      <c r="AJ50" s="13"/>
+      <c r="AK50" s="13"/>
+      <c r="AL50" s="14"/>
+      <c r="AM50" s="12"/>
+      <c r="AN50" s="13"/>
+      <c r="AO50" s="13"/>
+      <c r="AP50" s="14"/>
+      <c r="AQ50" s="12"/>
+      <c r="AR50" s="13"/>
+      <c r="AS50" s="13"/>
+      <c r="AT50" s="14"/>
+      <c r="AU50" s="12"/>
+      <c r="AV50" s="13"/>
+      <c r="AW50" s="13"/>
+      <c r="AX50" s="14"/>
+      <c r="AY50" s="12"/>
+      <c r="AZ50" s="13"/>
+      <c r="BA50" s="13"/>
+      <c r="BB50" s="14"/>
+      <c r="BC50" s="12"/>
+      <c r="BD50" s="13"/>
+      <c r="BE50" s="13"/>
+      <c r="BF50" s="14"/>
+      <c r="BG50" s="12"/>
+      <c r="BH50" s="13"/>
+      <c r="BI50" s="13"/>
+      <c r="BJ50" s="14"/>
+    </row>
+    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A51" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="52">
+        <v>6</v>
+      </c>
+      <c r="C51" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="56"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="74"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="74"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="10"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="11"/>
+      <c r="AA51" s="74"/>
+      <c r="AB51" s="10"/>
+      <c r="AC51" s="10"/>
+      <c r="AD51" s="11"/>
+      <c r="AE51" s="9"/>
+      <c r="AF51" s="10"/>
+      <c r="AG51" s="10"/>
+      <c r="AH51" s="11"/>
+      <c r="AI51" s="9"/>
+      <c r="AJ51" s="10"/>
+      <c r="AK51" s="10"/>
+      <c r="AL51" s="11"/>
+      <c r="AM51" s="9"/>
+      <c r="AN51" s="10"/>
+      <c r="AO51" s="10"/>
+      <c r="AP51" s="11"/>
+      <c r="AQ51" s="9"/>
+      <c r="AR51" s="10"/>
+      <c r="AS51" s="10"/>
+      <c r="AT51" s="11"/>
+      <c r="AU51" s="9"/>
+      <c r="AV51" s="10"/>
+      <c r="AW51" s="10"/>
+      <c r="AX51" s="11"/>
+      <c r="AY51" s="9"/>
+      <c r="AZ51" s="10"/>
+      <c r="BA51" s="10"/>
+      <c r="BB51" s="11"/>
+      <c r="BC51" s="9"/>
+      <c r="BD51" s="10"/>
+      <c r="BE51" s="10"/>
+      <c r="BF51" s="11"/>
+      <c r="BG51" s="9"/>
+      <c r="BH51" s="10"/>
+      <c r="BI51" s="10"/>
+      <c r="BJ51" s="11"/>
+    </row>
+    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A52" s="65"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="12"/>
+      <c r="X52" s="13"/>
+      <c r="Y52" s="13"/>
+      <c r="Z52" s="14"/>
+      <c r="AA52" s="12"/>
+      <c r="AB52" s="13"/>
+      <c r="AC52" s="13"/>
+      <c r="AD52" s="14"/>
+      <c r="AE52" s="12"/>
+      <c r="AF52" s="13"/>
+      <c r="AG52" s="13"/>
+      <c r="AH52" s="14"/>
+      <c r="AI52" s="12"/>
+      <c r="AJ52" s="13"/>
+      <c r="AK52" s="13"/>
+      <c r="AL52" s="14"/>
+      <c r="AM52" s="12"/>
+      <c r="AN52" s="13"/>
+      <c r="AO52" s="13"/>
+      <c r="AP52" s="14"/>
+      <c r="AQ52" s="12"/>
+      <c r="AR52" s="13"/>
+      <c r="AS52" s="13"/>
+      <c r="AT52" s="14"/>
+      <c r="AU52" s="12"/>
+      <c r="AV52" s="13"/>
+      <c r="AW52" s="13"/>
+      <c r="AX52" s="14"/>
+      <c r="AY52" s="12"/>
+      <c r="AZ52" s="13"/>
+      <c r="BA52" s="13"/>
+      <c r="BB52" s="14"/>
+      <c r="BC52" s="12"/>
+      <c r="BD52" s="13"/>
+      <c r="BE52" s="13"/>
+      <c r="BF52" s="14"/>
+      <c r="BG52" s="12"/>
+      <c r="BH52" s="13"/>
+      <c r="BI52" s="13"/>
+      <c r="BJ52" s="14"/>
+    </row>
+    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A53" s="65"/>
+      <c r="B53" s="52"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="76"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="40"/>
+      <c r="V53" s="78"/>
+      <c r="W53" s="45"/>
+      <c r="X53" s="40"/>
+      <c r="Y53" s="40"/>
+      <c r="Z53" s="78"/>
+      <c r="AA53" s="12"/>
+      <c r="AB53" s="13"/>
+      <c r="AC53" s="13"/>
+      <c r="AD53" s="14"/>
+      <c r="AE53" s="12"/>
+      <c r="AF53" s="13"/>
+      <c r="AG53" s="13"/>
+      <c r="AH53" s="14"/>
+      <c r="AI53" s="12"/>
+      <c r="AJ53" s="13"/>
+      <c r="AK53" s="13"/>
+      <c r="AL53" s="14"/>
+      <c r="AM53" s="12"/>
+      <c r="AN53" s="13"/>
+      <c r="AO53" s="13"/>
+      <c r="AP53" s="14"/>
+      <c r="AQ53" s="12"/>
+      <c r="AR53" s="13"/>
+      <c r="AS53" s="13"/>
+      <c r="AT53" s="14"/>
+      <c r="AU53" s="12"/>
+      <c r="AV53" s="13"/>
+      <c r="AW53" s="13"/>
+      <c r="AX53" s="14"/>
+      <c r="AY53" s="12"/>
+      <c r="AZ53" s="13"/>
+      <c r="BA53" s="13"/>
+      <c r="BB53" s="14"/>
+      <c r="BC53" s="12"/>
+      <c r="BD53" s="13"/>
+      <c r="BE53" s="13"/>
+      <c r="BF53" s="14"/>
+      <c r="BG53" s="12"/>
+      <c r="BH53" s="13"/>
+      <c r="BI53" s="13"/>
+      <c r="BJ53" s="14"/>
+    </row>
+    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A54" s="66"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="12"/>
+      <c r="T54" s="13"/>
+      <c r="U54" s="13"/>
+      <c r="V54" s="80"/>
+      <c r="W54" s="81"/>
+      <c r="X54" s="17"/>
+      <c r="Y54" s="17"/>
+      <c r="Z54" s="80"/>
+      <c r="AA54" s="12"/>
+      <c r="AB54" s="13"/>
+      <c r="AC54" s="13"/>
+      <c r="AD54" s="14"/>
+      <c r="AE54" s="12"/>
+      <c r="AF54" s="13"/>
+      <c r="AG54" s="13"/>
+      <c r="AH54" s="14"/>
+      <c r="AI54" s="12"/>
+      <c r="AJ54" s="13"/>
+      <c r="AK54" s="13"/>
+      <c r="AL54" s="14"/>
+      <c r="AM54" s="12"/>
+      <c r="AN54" s="13"/>
+      <c r="AO54" s="13"/>
+      <c r="AP54" s="14"/>
+      <c r="AQ54" s="12"/>
+      <c r="AR54" s="13"/>
+      <c r="AS54" s="13"/>
+      <c r="AT54" s="14"/>
+      <c r="AU54" s="12"/>
+      <c r="AV54" s="13"/>
+      <c r="AW54" s="13"/>
+      <c r="AX54" s="14"/>
+      <c r="AY54" s="12"/>
+      <c r="AZ54" s="13"/>
+      <c r="BA54" s="13"/>
+      <c r="BB54" s="14"/>
+      <c r="BC54" s="12"/>
+      <c r="BD54" s="13"/>
+      <c r="BE54" s="13"/>
+      <c r="BF54" s="14"/>
+      <c r="BG54" s="12"/>
+      <c r="BH54" s="13"/>
+      <c r="BI54" s="13"/>
+      <c r="BJ54" s="14"/>
+    </row>
+    <row r="55" spans="1:62" ht="21" x14ac:dyDescent="0.25">
+      <c r="A55" s="62"/>
+      <c r="B55" s="70">
         <v>11</v>
       </c>
-      <c r="C27" s="68" t="s">
+      <c r="C55" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="36" t="s">
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="30"/>
+      <c r="O55" s="28"/>
+      <c r="P55" s="29"/>
+      <c r="Q55" s="29"/>
+      <c r="R55" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="S27" s="29"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="29"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="31"/>
-      <c r="AA27" s="29"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="31"/>
-      <c r="AE27" s="29"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="31" t="s">
+      <c r="S55" s="28"/>
+      <c r="T55" s="29"/>
+      <c r="U55" s="29"/>
+      <c r="V55" s="30"/>
+      <c r="W55" s="28"/>
+      <c r="X55" s="29"/>
+      <c r="Y55" s="29"/>
+      <c r="Z55" s="30"/>
+      <c r="AA55" s="28"/>
+      <c r="AB55" s="29"/>
+      <c r="AC55" s="29"/>
+      <c r="AD55" s="30"/>
+      <c r="AE55" s="28"/>
+      <c r="AF55" s="29"/>
+      <c r="AG55" s="29"/>
+      <c r="AH55" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AI27" s="29"/>
-      <c r="AJ27" s="30"/>
-      <c r="AK27" s="30"/>
-      <c r="AL27" s="31"/>
-      <c r="AM27" s="29"/>
-      <c r="AN27" s="30"/>
-      <c r="AO27" s="30"/>
-      <c r="AP27" s="31"/>
-      <c r="AQ27" s="29"/>
-      <c r="AR27" s="30"/>
-      <c r="AS27" s="30"/>
-      <c r="AT27" s="31"/>
-      <c r="AU27" s="29"/>
-      <c r="AV27" s="30"/>
-      <c r="AW27" s="30"/>
-      <c r="AX27" s="31"/>
-      <c r="AY27" s="29"/>
-      <c r="AZ27" s="30"/>
-      <c r="BA27" s="30"/>
-      <c r="BB27" s="31"/>
-      <c r="BC27" s="29"/>
-      <c r="BD27" s="30"/>
-      <c r="BE27" s="30"/>
-      <c r="BF27" s="31"/>
-      <c r="BG27" s="29"/>
-      <c r="BH27" s="30"/>
-      <c r="BI27" s="30"/>
-      <c r="BJ27" s="31"/>
-    </row>
-    <row r="28" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="35"/>
-      <c r="AA28" s="33"/>
-      <c r="AB28" s="34"/>
-      <c r="AC28" s="34"/>
-      <c r="AD28" s="35"/>
-      <c r="AE28" s="33"/>
-      <c r="AF28" s="34"/>
-      <c r="AG28" s="34"/>
-      <c r="AH28" s="35"/>
-      <c r="AI28" s="33"/>
-      <c r="AJ28" s="34"/>
-      <c r="AK28" s="34"/>
-      <c r="AL28" s="35"/>
-      <c r="AM28" s="33"/>
-      <c r="AN28" s="34"/>
-      <c r="AO28" s="34"/>
-      <c r="AP28" s="35"/>
-      <c r="AQ28" s="33"/>
-      <c r="AR28" s="34"/>
-      <c r="AS28" s="34"/>
-      <c r="AT28" s="35"/>
-      <c r="AU28" s="33"/>
-      <c r="AV28" s="34"/>
-      <c r="AW28" s="34"/>
-      <c r="AX28" s="35"/>
-      <c r="AY28" s="33"/>
-      <c r="AZ28" s="34"/>
-      <c r="BA28" s="34"/>
-      <c r="BB28" s="35"/>
-      <c r="BC28" s="33"/>
-      <c r="BD28" s="34"/>
-      <c r="BE28" s="34"/>
-      <c r="BF28" s="35"/>
-      <c r="BG28" s="33"/>
-      <c r="BH28" s="34"/>
-      <c r="BI28" s="34"/>
-      <c r="BJ28" s="35"/>
+      <c r="AI55" s="28"/>
+      <c r="AJ55" s="29"/>
+      <c r="AK55" s="29"/>
+      <c r="AL55" s="30"/>
+      <c r="AM55" s="28"/>
+      <c r="AN55" s="29"/>
+      <c r="AO55" s="29"/>
+      <c r="AP55" s="30"/>
+      <c r="AQ55" s="28"/>
+      <c r="AR55" s="29"/>
+      <c r="AS55" s="29"/>
+      <c r="AT55" s="30"/>
+      <c r="AU55" s="28"/>
+      <c r="AV55" s="29"/>
+      <c r="AW55" s="29"/>
+      <c r="AX55" s="30"/>
+      <c r="AY55" s="28"/>
+      <c r="AZ55" s="29"/>
+      <c r="BA55" s="29"/>
+      <c r="BB55" s="30"/>
+      <c r="BC55" s="28"/>
+      <c r="BD55" s="29"/>
+      <c r="BE55" s="29"/>
+      <c r="BF55" s="30"/>
+      <c r="BG55" s="28"/>
+      <c r="BH55" s="29"/>
+      <c r="BI55" s="29"/>
+      <c r="BJ55" s="30"/>
+    </row>
+    <row r="56" spans="1:62" ht="21" x14ac:dyDescent="0.25">
+      <c r="A56" s="63"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="32"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="34"/>
+      <c r="O56" s="32"/>
+      <c r="P56" s="33"/>
+      <c r="Q56" s="33"/>
+      <c r="R56" s="34"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="33"/>
+      <c r="U56" s="33"/>
+      <c r="V56" s="34"/>
+      <c r="W56" s="32"/>
+      <c r="X56" s="33"/>
+      <c r="Y56" s="33"/>
+      <c r="Z56" s="34"/>
+      <c r="AA56" s="32"/>
+      <c r="AB56" s="33"/>
+      <c r="AC56" s="33"/>
+      <c r="AD56" s="34"/>
+      <c r="AE56" s="32"/>
+      <c r="AF56" s="33"/>
+      <c r="AG56" s="33"/>
+      <c r="AH56" s="34"/>
+      <c r="AI56" s="32"/>
+      <c r="AJ56" s="33"/>
+      <c r="AK56" s="33"/>
+      <c r="AL56" s="34"/>
+      <c r="AM56" s="32"/>
+      <c r="AN56" s="33"/>
+      <c r="AO56" s="33"/>
+      <c r="AP56" s="34"/>
+      <c r="AQ56" s="32"/>
+      <c r="AR56" s="33"/>
+      <c r="AS56" s="33"/>
+      <c r="AT56" s="34"/>
+      <c r="AU56" s="32"/>
+      <c r="AV56" s="33"/>
+      <c r="AW56" s="33"/>
+      <c r="AX56" s="34"/>
+      <c r="AY56" s="32"/>
+      <c r="AZ56" s="33"/>
+      <c r="BA56" s="33"/>
+      <c r="BB56" s="34"/>
+      <c r="BC56" s="32"/>
+      <c r="BD56" s="33"/>
+      <c r="BE56" s="33"/>
+      <c r="BF56" s="34"/>
+      <c r="BG56" s="32"/>
+      <c r="BH56" s="33"/>
+      <c r="BI56" s="33"/>
+      <c r="BJ56" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="BG1:BJ1"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:E18"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
+  <mergeCells count="62">
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="A7:A46"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="D35:E38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:E22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:E14"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D23:E26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:E30"/>
+    <mergeCell ref="B55:B56"/>
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="AA1:AD1"/>
@@ -2619,11 +4432,36 @@
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D3:E6"/>
-    <mergeCell ref="D23:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:E22"/>
+    <mergeCell ref="D51:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:E56"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="AQ1:AT1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="BG1:BJ1"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E14"/>
+    <mergeCell ref="B47:B50"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>